<commit_message>
Changed start date for dim_calendar, small changes in the fct_portfolio_snapshots_daily
</commit_message>
<xml_diff>
--- a/seeds/raw_ticker_seed.xlsx
+++ b/seeds/raw_ticker_seed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1866,85 +1866,57 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>NVDA.US</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>NVDA</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>GROWTH</t>
-        </is>
-      </c>
+          <t>MNST.US</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>O.US</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>REAL_ESTATE</t>
-        </is>
-      </c>
+          <t>MSFT.US</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>OUJP11</t>
+          <t>NVDA.US</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>OUJP11</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
+          <t>GROWTH</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>OUJP12</t>
+          <t>O.US</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>OUJP11</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1952,72 +1924,76 @@
           <t>REAL_ESTATE</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>OXY.US</t>
+          <t>OUJP11</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>OXY</t>
+          <t>OUJP11</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>GROWTH</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
+          <t>REAL_ESTATE</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>PFE.US</t>
+          <t>OUJP12</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>OUJP11</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>GROWTH</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
+          <t>REAL_ESTATE</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>PFRM3</t>
+          <t>OXY.US</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>PFRM3</t>
+          <t>OXY</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2025,26 +2001,22 @@
           <t>GROWTH</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>PLTR.US</t>
+          <t>PFE.US</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>PLTR</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2062,17 +2034,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>RBRP11</t>
+          <t>PFRM3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>RBRP11</t>
+          <t>PFRM3</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
+          <t>GROWTH</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2089,39 +2061,35 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>RBRP12</t>
+          <t>PLTR.US</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>RBRP11</t>
+          <t>PLTR</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
+          <t>GROWTH</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>RECR11</t>
+          <t>RBRP11</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>RECR11</t>
+          <t>RBRP11</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2143,12 +2111,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>RECR12</t>
+          <t>RBRP12</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>RECR11</t>
+          <t>RBRP11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2170,17 +2138,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SAPR11</t>
+          <t>RECR11</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>SAPR11</t>
+          <t>RECR11</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GROWTH</t>
+          <t>REAL_ESTATE</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2197,17 +2165,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SOJA3</t>
+          <t>RECR12</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>SOJA3</t>
+          <t>RECR11</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>GROWTH</t>
+          <t>REAL_ESTATE</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2224,12 +2192,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SQIA3</t>
+          <t>SAPR11</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>SQIA3</t>
+          <t>SAPR11</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2251,12 +2219,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>STBP3</t>
+          <t>SOJA3</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>STBP3</t>
+          <t>SOJA3</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2278,12 +2246,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>SXRV.DE</t>
+          <t>SQIA3</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SXRV</t>
+          <t>SQIA3</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2293,96 +2261,100 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TESOURO IPCA+ COM JUROS SEMESTRAIS 2035</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+          <t>STBP3</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>STBP3</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>GROWTH</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>TESOURO SELIC 2025</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+          <t>SXRV.DE</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>SXRV</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>GROWTH</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>TIET11</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>TIET11</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>GROWTH</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
+          <t>TESOURO IPCA+ COM JUROS SEMESTRAIS 2035</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>TTD.US</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>TTD</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>GROWTH</t>
-        </is>
-      </c>
+          <t>TESOURO SELIC 2025</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
+      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>TTE.FR</t>
+          <t>TIET11</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>TTE</t>
+          <t>TIET11</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2392,24 +2364,24 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>UNIP6</t>
+          <t>TTD.US</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>UNIP6</t>
+          <t>TTD</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2417,26 +2389,22 @@
           <t>GROWTH</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>VALE3</t>
+          <t>TTE.FR</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>VALE3</t>
+          <t>TTE</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2446,51 +2414,51 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>VHYD.UK</t>
+          <t>UNIP6</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>VHYD</t>
+          <t>UNIP6</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>DEFENSIVE</t>
+          <t>GROWTH</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>VIIA3</t>
+          <t>VALE3</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>VIIA3</t>
+          <t>VALE3</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2512,44 +2480,44 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>VILG11</t>
+          <t>VHYD.UK</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>VILG11</t>
+          <t>VHYD</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
+          <t>DEFENSIVE</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GB</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>VRTA11</t>
+          <t>VIIA3</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>VRTA11</t>
+          <t>VIIA3</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
+          <t>GROWTH</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2566,12 +2534,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>VRTA12</t>
+          <t>VILG11</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>VRTA11</t>
+          <t>VILG11</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2593,17 +2561,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>VVAR3</t>
+          <t>VRTA11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>VIIA3</t>
+          <t>VRTA11</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>GROWTH</t>
+          <t>REAL_ESTATE</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2620,12 +2588,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>WDP.BE</t>
+          <t>VRTA12</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>WDP</t>
+          <t>VRTA11</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2635,29 +2603,29 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>BR</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>XPLG11</t>
+          <t>VVAR3</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>XPLG11</t>
+          <t>VIIA3</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>REAL_ESTATE</t>
+          <t>GROWTH</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2674,12 +2642,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>XPLG12</t>
+          <t>WDP.BE</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>XPLG11</t>
+          <t>WDP</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2689,24 +2657,24 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BE</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>XPML11</t>
+          <t>XPLG11</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>XPML11</t>
+          <t>XPLG11</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2728,25 +2696,79 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>XPLG12</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>XPLG11</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>REAL_ESTATE</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>XPML11</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>XPML11</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>REAL_ESTATE</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
           <t>XPML12</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B91" t="inlineStr">
         <is>
           <t>XPML11</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>REAL_ESTATE</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>REAL_ESTATE</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
         <is>
           <t>BR</t>
         </is>

</xml_diff>